<commit_message>
Linear Progamming Examples Using Excel Solver
</commit_message>
<xml_diff>
--- a/Linear Programming/LP Demos.xlsx
+++ b/Linear Programming/LP Demos.xlsx
@@ -5,122 +5,348 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\BARRQNAP01\home\Northwestern MSDS\MSDS 460 (Decision Analytics)\Extras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\BARRQNAP01\home\repos\Data-Science-Portfolio\Linear Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9471D7D-27A7-4C4C-B75B-5FCA3CC3A953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD199C4-AFD1-40A1-BC81-A247B80A3A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{942EF3DA-A3C1-4FB2-A2EF-866453224C28}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="5" activeTab="8" xr2:uid="{942EF3DA-A3C1-4FB2-A2EF-866453224C28}"/>
   </bookViews>
   <sheets>
     <sheet name="Max Profit - Soft Drinks" sheetId="1" r:id="rId1"/>
-    <sheet name="Max Profit - Hot Tub" sheetId="3" r:id="rId2"/>
-    <sheet name="Min - Cost Diet" sheetId="5" r:id="rId3"/>
-    <sheet name="Max Profit - Food startup" sheetId="7" r:id="rId4"/>
+    <sheet name="Max Profit - Clothing" sheetId="8" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="10" r:id="rId3"/>
+    <sheet name="Max Revenue - New Stores" sheetId="11" r:id="rId4"/>
+    <sheet name="Max Profit - Hot Tub" sheetId="3" r:id="rId5"/>
+    <sheet name="Min - Cost Diet" sheetId="5" r:id="rId6"/>
+    <sheet name="Max Profit - Food startup" sheetId="7" r:id="rId7"/>
+    <sheet name="Max Profit - Two Models" sheetId="12" r:id="rId8"/>
+    <sheet name="Min - Simple Transport" sheetId="15" r:id="rId9"/>
+    <sheet name="Min - Trasnsport Refridgerators" sheetId="13" r:id="rId10"/>
+    <sheet name="Min - Transport OJ" sheetId="14" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">'Max Profit - Food startup'!$Q$4:$S$4</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Max Profit - Hot Tub'!$C$4:$D$4</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Max Profit - Clothing'!$C$18:$D$18</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'Max Profit - Food startup'!$Q$4:$S$4</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'Max Profit - Hot Tub'!$C$4:$D$4</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Max Profit - Soft Drinks'!$E$18:$F$18</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'Min - Cost Diet'!$N$4:$Q$4</definedName>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">'Max Profit - Two Models'!$I$18:$J$18</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'Max Revenue - New Stores'!$C$24:$E$24</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'Min - Cost Diet'!$N$4:$Q$4</definedName>
+    <definedName name="solver_adj" localSheetId="8" hidden="1">'Min - Simple Transport'!$P$14:$U$14</definedName>
+    <definedName name="solver_adj" localSheetId="10" hidden="1">'Min - Transport OJ'!$C$24:$K$24</definedName>
+    <definedName name="solver_adj" localSheetId="9" hidden="1">'Min - Trasnsport Refridgerators'!$C$17:$F$17</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Sheet3!$C$10:$D$10</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="8" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="10" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="9" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="8" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="8" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="10" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Max Profit - Food startup'!$T$11:$T$16</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Max Profit - Hot Tub'!$E$9:$E$11</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Max Profit - Clothing'!$E$23:$E$24</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'Max Profit - Food startup'!$T$11:$T$16</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'Max Profit - Hot Tub'!$E$9:$E$11</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Max Profit - Soft Drinks'!$G$25:$G$27</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Min - Cost Diet'!$R$11:$R$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">'Max Profit - Two Models'!$K$23:$K$24</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Max Revenue - New Stores'!$F$30:$F$32</definedName>
+    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'Min - Cost Diet'!$R$11:$R$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="8" hidden="1">'Min - Simple Transport'!$V$21:$V$25</definedName>
+    <definedName name="solver_lhs1" localSheetId="10" hidden="1">'Min - Transport OJ'!$L$31:$L$33</definedName>
+    <definedName name="solver_lhs1" localSheetId="9" hidden="1">'Min - Trasnsport Refridgerators'!$G$23:$G$26</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">Sheet3!$E$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="10" hidden="1">'Min - Transport OJ'!$L$34:$L$36</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">Sheet3!$E$17:$E$18</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">Sheet3!$E$19</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="8" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="10" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="8" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="10" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="9" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="8" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="10" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="9" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="8" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="8" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="10" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="9" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="9" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">'Max Profit - Food startup'!$V$7</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Max Profit - Hot Tub'!$G$6</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Max Profit - Clothing'!$G$20</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'Max Profit - Food startup'!$V$7</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'Max Profit - Hot Tub'!$G$6</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Max Profit - Soft Drinks'!$I$21</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'Min - Cost Diet'!$T$7</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">'Max Profit - Two Models'!$M$20</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'Max Revenue - New Stores'!$H$26</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'Min - Cost Diet'!$T$7</definedName>
+    <definedName name="solver_opt" localSheetId="8" hidden="1">'Min - Simple Transport'!$Y$17</definedName>
+    <definedName name="solver_opt" localSheetId="10" hidden="1">'Min - Transport OJ'!$N$27</definedName>
+    <definedName name="solver_opt" localSheetId="9" hidden="1">'Min - Trasnsport Refridgerators'!$I$20</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Sheet3!$G$13</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="8" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="10" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="9" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'Max Profit - Food startup'!$V$11:$V$16</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Max Profit - Hot Tub'!$G$9:$G$11</definedName>
+    <definedName name="solver_rel1" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="8" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="10" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="9" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Max Profit - Clothing'!$G$23:$G$24</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">'Max Profit - Food startup'!$V$11:$V$16</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">'Max Profit - Hot Tub'!$G$9:$G$11</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Max Profit - Soft Drinks'!$I$25:$I$27</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'Min - Cost Diet'!$T$11:$T$14</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">'Max Profit - Two Models'!$M$23:$M$24</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'Max Revenue - New Stores'!$H$30:$H$32</definedName>
+    <definedName name="solver_rhs1" localSheetId="5" hidden="1">'Min - Cost Diet'!$T$11:$T$14</definedName>
+    <definedName name="solver_rhs1" localSheetId="8" hidden="1">'Min - Simple Transport'!$X$21:$X$25</definedName>
+    <definedName name="solver_rhs1" localSheetId="10" hidden="1">'Min - Transport OJ'!$N$31:$N$33</definedName>
+    <definedName name="solver_rhs1" localSheetId="9" hidden="1">'Min - Trasnsport Refridgerators'!$I$23:$I$26</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">Sheet3!$G$16</definedName>
+    <definedName name="solver_rhs2" localSheetId="10" hidden="1">'Min - Transport OJ'!$N$34:$N$36</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">Sheet3!$G$17:$G$18</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">Sheet3!$G$19</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="8" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="10" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="9" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="8" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="9" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="8" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="10" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="9" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="8" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="10" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="9" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="8" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="10" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="9" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="8" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="10" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="9" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="10" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="9" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="8" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="10" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="9" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -142,7 +368,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="204">
   <si>
     <t>Decision Variables</t>
   </si>
@@ -469,13 +695,298 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Decision Variable</t>
+  </si>
+  <si>
+    <t>Var Value (Chaning variable)</t>
+  </si>
+  <si>
+    <t>Object Function</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Dresses</t>
+  </si>
+  <si>
+    <t>Trousers</t>
+  </si>
+  <si>
+    <t>Max Profit</t>
+  </si>
+  <si>
+    <t>C1: Minutes of Cutting</t>
+  </si>
+  <si>
+    <t>C2: Minutes of Stitching</t>
+  </si>
+  <si>
+    <t>Var Value (Changing Variable)</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Cabbage</t>
+  </si>
+  <si>
+    <t>C3: Cabbage</t>
+  </si>
+  <si>
+    <t>C1: Acrage</t>
+  </si>
+  <si>
+    <t>C2: Corn</t>
+  </si>
+  <si>
+    <t>C4: cabbage &gt;= 3*corn</t>
+  </si>
+  <si>
+    <t>Conveniene Store</t>
+  </si>
+  <si>
+    <t>Standard Store</t>
+  </si>
+  <si>
+    <t>Expanded Services Store</t>
+  </si>
+  <si>
+    <t>Contraings</t>
+  </si>
+  <si>
+    <t>C1: Building Cost</t>
+  </si>
+  <si>
+    <t>C2: Employees to Run</t>
+  </si>
+  <si>
+    <t>C3: Number of building to build</t>
+  </si>
+  <si>
+    <t>Decisiono Variables</t>
+  </si>
+  <si>
+    <t>Model1</t>
+  </si>
+  <si>
+    <t>Model2</t>
+  </si>
+  <si>
+    <t>C1: Grinding Hours</t>
+  </si>
+  <si>
+    <t>C2: Polishing Hours</t>
+  </si>
+  <si>
+    <t>Store X</t>
+  </si>
+  <si>
+    <t>Store Y</t>
+  </si>
+  <si>
+    <t>Warehouse A</t>
+  </si>
+  <si>
+    <t>Warehouse B</t>
+  </si>
+  <si>
+    <t>50x1</t>
+  </si>
+  <si>
+    <t>60x2</t>
+  </si>
+  <si>
+    <t>50x3</t>
+  </si>
+  <si>
+    <t>40x4</t>
+  </si>
+  <si>
+    <t>Decsion Variables</t>
+  </si>
+  <si>
+    <t>AX (x1)</t>
+  </si>
+  <si>
+    <t>AY (x2)</t>
+  </si>
+  <si>
+    <t>BX (x3)</t>
+  </si>
+  <si>
+    <t>BY (x4)</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>C1: Store X</t>
+  </si>
+  <si>
+    <t>C2: Store Y</t>
+  </si>
+  <si>
+    <t>C3: Warehouse A</t>
+  </si>
+  <si>
+    <t>C4: Warehouse B</t>
+  </si>
+  <si>
+    <t>Ocala</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Leesburg</t>
+  </si>
+  <si>
+    <t>Mt. Dora</t>
+  </si>
+  <si>
+    <t>Eustis</t>
+  </si>
+  <si>
+    <t>Clermont</t>
+  </si>
+  <si>
+    <t>21x1</t>
+  </si>
+  <si>
+    <t>50x2</t>
+  </si>
+  <si>
+    <t>40x3</t>
+  </si>
+  <si>
+    <t>35x4</t>
+  </si>
+  <si>
+    <t>30x5</t>
+  </si>
+  <si>
+    <t>22x6</t>
+  </si>
+  <si>
+    <t>55x7</t>
+  </si>
+  <si>
+    <t>20x8</t>
+  </si>
+  <si>
+    <t>25x9</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t>x5</t>
+  </si>
+  <si>
+    <t>x6</t>
+  </si>
+  <si>
+    <t>x7</t>
+  </si>
+  <si>
+    <t>x8</t>
+  </si>
+  <si>
+    <t>x9</t>
+  </si>
+  <si>
+    <t>C1: Ocal Capacity</t>
+  </si>
+  <si>
+    <t>C2: Orlando Capacity</t>
+  </si>
+  <si>
+    <t>C3: Leesburg Capacity</t>
+  </si>
+  <si>
+    <t>C4: Mt. Dora Bushels</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>C5: Eustis Bushels</t>
+  </si>
+  <si>
+    <t>C6: Clermont Bushels</t>
+  </si>
+  <si>
+    <t>Plant A</t>
+  </si>
+  <si>
+    <t>Plant B</t>
+  </si>
+  <si>
+    <t>4x1</t>
+  </si>
+  <si>
+    <t>6x2</t>
+  </si>
+  <si>
+    <t>4x3</t>
+  </si>
+  <si>
+    <t>6x4</t>
+  </si>
+  <si>
+    <t>5x5</t>
+  </si>
+  <si>
+    <t>2x6</t>
+  </si>
+  <si>
+    <t>Var Value (Changing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective </t>
+  </si>
+  <si>
+    <t>C1: Plant A at least 60 units</t>
+  </si>
+  <si>
+    <t>C2: Plant B at least 60 Units</t>
+  </si>
+  <si>
+    <t>DC1</t>
+  </si>
+  <si>
+    <t>DC2</t>
+  </si>
+  <si>
+    <t>DC3</t>
+  </si>
+  <si>
+    <t>C3: D1</t>
+  </si>
+  <si>
+    <t>C4: D2</t>
+  </si>
+  <si>
+    <t>C5: D3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,8 +1009,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -539,6 +1056,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,7 +1116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -620,6 +1143,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,6 +1230,201 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61828AF5-8D41-4B20-951C-4A0D94FF5981}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="209551"/>
+          <a:ext cx="12868275" cy="1904999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A small business enterprise makes dresses and trousers. To make a dress requires 1/2 hour of cutting and 20 minutes of stitching. To make a trousers requires 15 minutes of cutting and 1/2 hour of stitching. The profit on a dress is $40 and on a pair of trousers $50. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The business operates for a maximum of 8 hours per day.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Determine how many dresses and trousers should be made to maximize profit and what the maximum profit is ...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>525045</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9994</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD6AB8B1-5048-476B-BAF0-34D2770A4AB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="76200"/>
+          <a:ext cx="8383170" cy="3362794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -770,7 +1503,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -814,6 +1547,1397 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07053F9D-0143-45ED-8A0F-8695A77CA124}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619126" y="180975"/>
+          <a:ext cx="7905750" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A manufacturer produces two models M1 and M2 product. Each unit of model M1 requires 4 hours grinding and 2 hours polishing. Each unit of model M2 requires 2 hours grinding and 5 hours of polishing. The manufacturer has 2 grindings each of which works for 40 hours per week. There are 3 polishing each of which works for 60 hours per week. Profit on model M1 is Rs. 300 per unit and profit on model M2 is 400 per unit. The manufacturer has to allocate his production capacity so as to maximize his profit. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5425C4C1-E9E1-452D-ACD1-9B034F334B30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133351" y="152400"/>
+          <a:ext cx="6553199" cy="3552825"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 6553199"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 3552825"/>
+            <a:gd name="connsiteX1" fmla="*/ 6553199 w 6553199"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 3552825"/>
+            <a:gd name="connsiteX2" fmla="*/ 6553199 w 6553199"/>
+            <a:gd name="connsiteY2" fmla="*/ 3552825 h 3552825"/>
+            <a:gd name="connsiteX3" fmla="*/ 0 w 6553199"/>
+            <a:gd name="connsiteY3" fmla="*/ 3552825 h 3552825"/>
+            <a:gd name="connsiteX4" fmla="*/ 0 w 6553199"/>
+            <a:gd name="connsiteY4" fmla="*/ 0 h 3552825"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="6553199" h="3552825" fill="none" extrusionOk="0">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="757626" y="-49533"/>
+                <a:pt x="3439290" y="-14809"/>
+                <a:pt x="6553199" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="6640838" y="948911"/>
+                <a:pt x="6480520" y="1812593"/>
+                <a:pt x="6553199" y="3552825"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="5126639" y="3504594"/>
+                <a:pt x="1038136" y="3637280"/>
+                <a:pt x="0" y="3552825"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-38581" y="2714179"/>
+                <a:pt x="63341" y="562066"/>
+                <a:pt x="0" y="0"/>
+              </a:cubicBezTo>
+              <a:close/>
+            </a:path>
+            <a:path w="6553199" h="3552825" stroke="0" extrusionOk="0">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="1805958" y="118645"/>
+                <a:pt x="3743528" y="116012"/>
+                <a:pt x="6553199" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="6420317" y="1187034"/>
+                <a:pt x="6638150" y="2252944"/>
+                <a:pt x="6553199" y="3552825"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="4638574" y="3687425"/>
+                <a:pt x="2874556" y="3395629"/>
+                <a:pt x="0" y="3552825"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-20187" y="2856852"/>
+                <a:pt x="-152480" y="1483639"/>
+                <a:pt x="0" y="0"/>
+              </a:cubicBezTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:extLst>
+            <a:ext uri="{C807C97D-BFC1-408E-A445-0C87EB9F89A2}">
+              <ask:lineSketchStyleProps xmlns:ask="http://schemas.microsoft.com/office/drawing/2018/sketchyshapes" sd="1219033472">
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <ask:type>
+                  <ask:lineSketchCurved/>
+                </ask:type>
+              </ask:lineSketchStyleProps>
+            </a:ext>
+          </a:extLst>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A company has two plants producing a certain product that is to be shipped to three distribution centers. The unit production costs are the same at the two plants, and the shipping cost per unit is shown below.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	                   Distribution Center</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	1 	2 	3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Plant</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A 	$4	 $6	 $4</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>B	$6 	$5 	$2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Shipments are made once per week. During each week, each plant produces at most 60 units and each distribution center needs at least 40 units. How many units should be shipped from each plant to each distribution center, so as to minimize cost?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Arrow: Right 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AD62E6F-F13F-496F-B1A3-BDC9E3253C2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7124701" y="923925"/>
+          <a:ext cx="3448050" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89FCBF6C-4BB6-4F43-BD54-F828ADAD226C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="180975" y="85726"/>
+          <a:ext cx="7610475" cy="2209800"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 7610475"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX1" fmla="*/ 767966 w 7610475"/>
+            <a:gd name="connsiteY1" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX2" fmla="*/ 1383723 w 7610475"/>
+            <a:gd name="connsiteY2" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX3" fmla="*/ 2075584 w 7610475"/>
+            <a:gd name="connsiteY3" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX4" fmla="*/ 2919655 w 7610475"/>
+            <a:gd name="connsiteY4" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX5" fmla="*/ 3459307 w 7610475"/>
+            <a:gd name="connsiteY5" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX6" fmla="*/ 4227273 w 7610475"/>
+            <a:gd name="connsiteY6" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX7" fmla="*/ 4766925 w 7610475"/>
+            <a:gd name="connsiteY7" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX8" fmla="*/ 5458786 w 7610475"/>
+            <a:gd name="connsiteY8" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX9" fmla="*/ 6226752 w 7610475"/>
+            <a:gd name="connsiteY9" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX10" fmla="*/ 6690299 w 7610475"/>
+            <a:gd name="connsiteY10" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX11" fmla="*/ 7610475 w 7610475"/>
+            <a:gd name="connsiteY11" fmla="*/ 0 h 2209800"/>
+            <a:gd name="connsiteX12" fmla="*/ 7610475 w 7610475"/>
+            <a:gd name="connsiteY12" fmla="*/ 596646 h 2209800"/>
+            <a:gd name="connsiteX13" fmla="*/ 7610475 w 7610475"/>
+            <a:gd name="connsiteY13" fmla="*/ 1193292 h 2209800"/>
+            <a:gd name="connsiteX14" fmla="*/ 7610475 w 7610475"/>
+            <a:gd name="connsiteY14" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX15" fmla="*/ 6994718 w 7610475"/>
+            <a:gd name="connsiteY15" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX16" fmla="*/ 6378962 w 7610475"/>
+            <a:gd name="connsiteY16" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX17" fmla="*/ 5610996 w 7610475"/>
+            <a:gd name="connsiteY17" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX18" fmla="*/ 4919134 w 7610475"/>
+            <a:gd name="connsiteY18" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX19" fmla="*/ 4075063 w 7610475"/>
+            <a:gd name="connsiteY19" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX20" fmla="*/ 3230993 w 7610475"/>
+            <a:gd name="connsiteY20" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX21" fmla="*/ 2463026 w 7610475"/>
+            <a:gd name="connsiteY21" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX22" fmla="*/ 1695060 w 7610475"/>
+            <a:gd name="connsiteY22" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX23" fmla="*/ 927094 w 7610475"/>
+            <a:gd name="connsiteY23" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX24" fmla="*/ 0 w 7610475"/>
+            <a:gd name="connsiteY24" fmla="*/ 2209800 h 2209800"/>
+            <a:gd name="connsiteX25" fmla="*/ 0 w 7610475"/>
+            <a:gd name="connsiteY25" fmla="*/ 1613154 h 2209800"/>
+            <a:gd name="connsiteX26" fmla="*/ 0 w 7610475"/>
+            <a:gd name="connsiteY26" fmla="*/ 1060704 h 2209800"/>
+            <a:gd name="connsiteX27" fmla="*/ 0 w 7610475"/>
+            <a:gd name="connsiteY27" fmla="*/ 574548 h 2209800"/>
+            <a:gd name="connsiteX28" fmla="*/ 0 w 7610475"/>
+            <a:gd name="connsiteY28" fmla="*/ 0 h 2209800"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX5" y="connsiteY5"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX6" y="connsiteY6"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX7" y="connsiteY7"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX8" y="connsiteY8"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX9" y="connsiteY9"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX10" y="connsiteY10"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX11" y="connsiteY11"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX12" y="connsiteY12"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX13" y="connsiteY13"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX14" y="connsiteY14"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX15" y="connsiteY15"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX16" y="connsiteY16"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX17" y="connsiteY17"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX18" y="connsiteY18"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX19" y="connsiteY19"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX20" y="connsiteY20"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX21" y="connsiteY21"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX22" y="connsiteY22"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX23" y="connsiteY23"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX24" y="connsiteY24"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX25" y="connsiteY25"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX26" y="connsiteY26"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX27" y="connsiteY27"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX28" y="connsiteY28"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="7610475" h="2209800" fill="none" extrusionOk="0">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="160352" y="-15309"/>
+                <a:pt x="399764" y="-28253"/>
+                <a:pt x="767966" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1136168" y="28253"/>
+                <a:pt x="1150767" y="28687"/>
+                <a:pt x="1383723" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1616679" y="-28687"/>
+                <a:pt x="1832769" y="-16826"/>
+                <a:pt x="2075584" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2318399" y="16826"/>
+                <a:pt x="2540059" y="27731"/>
+                <a:pt x="2919655" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3299251" y="-27731"/>
+                <a:pt x="3227691" y="13358"/>
+                <a:pt x="3459307" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3690923" y="-13358"/>
+                <a:pt x="3909403" y="-15968"/>
+                <a:pt x="4227273" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="4545143" y="15968"/>
+                <a:pt x="4542341" y="186"/>
+                <a:pt x="4766925" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="4991509" y="-186"/>
+                <a:pt x="5244554" y="-15116"/>
+                <a:pt x="5458786" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="5673018" y="15116"/>
+                <a:pt x="6020604" y="-29969"/>
+                <a:pt x="6226752" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="6432900" y="29969"/>
+                <a:pt x="6459685" y="2514"/>
+                <a:pt x="6690299" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="6920913" y="-2514"/>
+                <a:pt x="7207318" y="-2965"/>
+                <a:pt x="7610475" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7606134" y="188939"/>
+                <a:pt x="7600664" y="444947"/>
+                <a:pt x="7610475" y="596646"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7620286" y="748345"/>
+                <a:pt x="7617294" y="931750"/>
+                <a:pt x="7610475" y="1193292"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7603656" y="1454834"/>
+                <a:pt x="7606376" y="1879678"/>
+                <a:pt x="7610475" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7365974" y="2224327"/>
+                <a:pt x="7155846" y="2191690"/>
+                <a:pt x="6994718" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="6833590" y="2227910"/>
+                <a:pt x="6582253" y="2239979"/>
+                <a:pt x="6378962" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="6175671" y="2179621"/>
+                <a:pt x="5823937" y="2209343"/>
+                <a:pt x="5610996" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="5398055" y="2210257"/>
+                <a:pt x="5092147" y="2209955"/>
+                <a:pt x="4919134" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="4746121" y="2209645"/>
+                <a:pt x="4332396" y="2185756"/>
+                <a:pt x="4075063" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3817730" y="2233844"/>
+                <a:pt x="3463589" y="2233458"/>
+                <a:pt x="3230993" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2998397" y="2186143"/>
+                <a:pt x="2713644" y="2188685"/>
+                <a:pt x="2463026" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2212408" y="2230915"/>
+                <a:pt x="2015057" y="2190250"/>
+                <a:pt x="1695060" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1375063" y="2229350"/>
+                <a:pt x="1276468" y="2209753"/>
+                <a:pt x="927094" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="577720" y="2209847"/>
+                <a:pt x="289769" y="2193488"/>
+                <a:pt x="0" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-14216" y="1918521"/>
+                <a:pt x="8027" y="1810564"/>
+                <a:pt x="0" y="1613154"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-8027" y="1415744"/>
+                <a:pt x="-27091" y="1312987"/>
+                <a:pt x="0" y="1060704"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="27091" y="808421"/>
+                <a:pt x="-1752" y="778408"/>
+                <a:pt x="0" y="574548"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1752" y="370688"/>
+                <a:pt x="-20217" y="233455"/>
+                <a:pt x="0" y="0"/>
+              </a:cubicBezTo>
+              <a:close/>
+            </a:path>
+            <a:path w="7610475" h="2209800" stroke="0" extrusionOk="0">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="218209" y="-25188"/>
+                <a:pt x="435735" y="-848"/>
+                <a:pt x="615757" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="795779" y="848"/>
+                <a:pt x="849667" y="19374"/>
+                <a:pt x="1079304" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1308941" y="-19374"/>
+                <a:pt x="1741158" y="-19752"/>
+                <a:pt x="1923375" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2105592" y="19752"/>
+                <a:pt x="2394520" y="6446"/>
+                <a:pt x="2539131" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2683742" y="-6446"/>
+                <a:pt x="2862865" y="29653"/>
+                <a:pt x="3154888" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3446911" y="-29653"/>
+                <a:pt x="3788661" y="21538"/>
+                <a:pt x="3998959" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="4209257" y="-21538"/>
+                <a:pt x="4334120" y="-5094"/>
+                <a:pt x="4538611" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="4743102" y="5094"/>
+                <a:pt x="5022369" y="12541"/>
+                <a:pt x="5382681" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="5742993" y="-12541"/>
+                <a:pt x="5860413" y="-30844"/>
+                <a:pt x="6226752" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="6593091" y="30844"/>
+                <a:pt x="6751253" y="-18320"/>
+                <a:pt x="6918614" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7085975" y="18320"/>
+                <a:pt x="7293569" y="-28262"/>
+                <a:pt x="7610475" y="0"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7614144" y="197613"/>
+                <a:pt x="7632961" y="287114"/>
+                <a:pt x="7610475" y="530352"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7587989" y="773590"/>
+                <a:pt x="7630254" y="794436"/>
+                <a:pt x="7610475" y="1016508"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7590696" y="1238580"/>
+                <a:pt x="7632714" y="1415161"/>
+                <a:pt x="7610475" y="1568958"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7588237" y="1722755"/>
+                <a:pt x="7627124" y="2028896"/>
+                <a:pt x="7610475" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="7407744" y="2180206"/>
+                <a:pt x="7197889" y="2228648"/>
+                <a:pt x="6918614" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="6639339" y="2190952"/>
+                <a:pt x="6466516" y="2214005"/>
+                <a:pt x="6074543" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="5682570" y="2205595"/>
+                <a:pt x="5628787" y="2217873"/>
+                <a:pt x="5382681" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="5136575" y="2201727"/>
+                <a:pt x="5013243" y="2205096"/>
+                <a:pt x="4919134" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="4825025" y="2214504"/>
+                <a:pt x="4504011" y="2198436"/>
+                <a:pt x="4379482" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="4254953" y="2221164"/>
+                <a:pt x="3748433" y="2216973"/>
+                <a:pt x="3535412" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="3322391" y="2202628"/>
+                <a:pt x="2983195" y="2229836"/>
+                <a:pt x="2843550" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2703905" y="2189764"/>
+                <a:pt x="2451628" y="2230640"/>
+                <a:pt x="2303898" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="2156168" y="2188960"/>
+                <a:pt x="1954085" y="2242680"/>
+                <a:pt x="1612037" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="1269989" y="2176920"/>
+                <a:pt x="1352274" y="2193086"/>
+                <a:pt x="1148490" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="944706" y="2226514"/>
+                <a:pt x="788801" y="2225957"/>
+                <a:pt x="684943" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="581085" y="2193643"/>
+                <a:pt x="212958" y="2189054"/>
+                <a:pt x="0" y="2209800"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-18028" y="1986040"/>
+                <a:pt x="15596" y="1953127"/>
+                <a:pt x="0" y="1701546"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="-15596" y="1449965"/>
+                <a:pt x="-15235" y="1316945"/>
+                <a:pt x="0" y="1104900"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="15235" y="892855"/>
+                <a:pt x="-12119" y="735444"/>
+                <a:pt x="0" y="574548"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="12119" y="413652"/>
+                <a:pt x="25088" y="209447"/>
+                <a:pt x="0" y="0"/>
+              </a:cubicBezTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="28575" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:extLst>
+            <a:ext uri="{C807C97D-BFC1-408E-A445-0C87EB9F89A2}">
+              <ask:lineSketchStyleProps xmlns:ask="http://schemas.microsoft.com/office/drawing/2018/sketchyshapes" sd="1219033472">
+                <a:prstGeom prst="rect">
+                  <a:avLst/>
+                </a:prstGeom>
+                <ask:type>
+                  <ask:lineSketchFreehand/>
+                </ask:type>
+              </ask:lineSketchStyleProps>
+            </a:ext>
+          </a:extLst>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A distributor receives orders for some new side-by-side refrigerators from stores X and Y. Those refrigerators are available in warehouses A and B. Store X needs at least 100 refrigerators, and Store Y needs at least 150 refrigerators. Warehouse A can supply at least 200 refrigerators, and Warehouse B can supply at least 100 refrigerators. It costs $50 per refrigerator to ship from A to X, $60 per refrigerator to ship from A to Y, $50 per refrigerator to ship from B to X, and $40 per refrigerator to ship from B to Y. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>How many refrigerators does the distributor send to the different</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>stores from which warehouse to fulfill the orders and minimize the total cost?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Arrow: Right 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DEB959C-0268-496E-9134-AB376EF7F12C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8001000" y="952500"/>
+          <a:ext cx="942975" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70489FAB-6FC6-479D-8CD4-C663084534E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="104775" y="85725"/>
+          <a:ext cx="7496175" cy="3514726"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="31750" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Tropicsun is a leading grower and distributor of fresh citrus products with three large citrus groves scattered around central Florida in the cities of Mt. Dora, Eustis, and Clermont. Tropicsun currently has 275,000 bushels of citrus at the grove in Mt.Dora, 400,000 bushels at the grove in Eustis, and 300,000 bushels at the grove in Clermont. Tropicsun has citrus processing plants in Ocala, Orlando, and Leesburg</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>with processing capacities to handle 200,000, 600,000, and 225,000 bushels, respectively. Tropicsun contracts with a local trucking company to transport its fruit from the groves to the processing plants. The trucking company charges a flat rate for every mile that each bushel of fruit must be transported. Each mile a bushel of fruit travels is known as a bushel-mile.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Distances (in miles) Between groves and Plants grove </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>                     Ocala Orlando Leesburg</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Mt. Dora         </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>21        50          40</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Eustis   </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>           35        30           22</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Clermont  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>      55        20           25</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Tropicsun wants to determine how many bushels to ship from each grove to</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>each processing plant in order to process all the fruit while minimizing the total</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>number of bushel-miles the fruit must be shipped</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Arrow: Right 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B920DC62-3645-4AED-87B7-6EF4B0B50935}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7915275" y="1543050"/>
+          <a:ext cx="1619250" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1118,7 +3242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB0A3E0-BFCA-4EC3-9902-E09C77364B10}">
   <dimension ref="C16:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -1465,7 +3589,1255 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1129200-B149-45EB-B196-3F674B251134}">
+  <dimension ref="A4:S26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>137</v>
+      </c>
+      <c r="R4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>141</v>
+      </c>
+      <c r="R5" t="s">
+        <v>142</v>
+      </c>
+      <c r="S5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>143</v>
+      </c>
+      <c r="R6" t="s">
+        <v>144</v>
+      </c>
+      <c r="S6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>100</v>
+      </c>
+      <c r="R7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="1">
+        <v>150</v>
+      </c>
+      <c r="D17" s="1">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2">
+        <v>50</v>
+      </c>
+      <c r="D20" s="2">
+        <v>60</v>
+      </c>
+      <c r="E20" s="2">
+        <v>50</v>
+      </c>
+      <c r="F20" s="2">
+        <v>40</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I20" s="3">
+        <f>SUMPRODUCT(C17:F17,C20:F20)</f>
+        <v>14500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f>SUMPRODUCT(C$17:F$17,C23:F23)</f>
+        <v>150</v>
+      </c>
+      <c r="H23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G26" si="0">SUMPRODUCT(C$17:F$17,C24:F24)</f>
+        <v>150</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H25" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H26" t="s">
+        <v>67</v>
+      </c>
+      <c r="I26">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B2F4B4-AE4C-46ED-A71F-691FB5728CA4}">
+  <dimension ref="A8:U41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>155</v>
+      </c>
+      <c r="S8" t="s">
+        <v>156</v>
+      </c>
+      <c r="T8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q9" t="s">
+        <v>158</v>
+      </c>
+      <c r="R9" t="s">
+        <v>161</v>
+      </c>
+      <c r="S9" t="s">
+        <v>162</v>
+      </c>
+      <c r="T9" t="s">
+        <v>163</v>
+      </c>
+      <c r="U9">
+        <v>275000</v>
+      </c>
+    </row>
+    <row r="10" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>159</v>
+      </c>
+      <c r="R10" t="s">
+        <v>164</v>
+      </c>
+      <c r="S10" t="s">
+        <v>165</v>
+      </c>
+      <c r="T10" t="s">
+        <v>166</v>
+      </c>
+      <c r="U10">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="11" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q11" t="s">
+        <v>160</v>
+      </c>
+      <c r="R11" t="s">
+        <v>167</v>
+      </c>
+      <c r="S11" t="s">
+        <v>168</v>
+      </c>
+      <c r="T11" t="s">
+        <v>169</v>
+      </c>
+      <c r="U11">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="12" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>200000</v>
+      </c>
+      <c r="S12">
+        <v>600000</v>
+      </c>
+      <c r="T12">
+        <v>225000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="19">
+        <v>200000</v>
+      </c>
+      <c r="D24" s="19">
+        <v>0</v>
+      </c>
+      <c r="E24" s="19">
+        <v>75000</v>
+      </c>
+      <c r="F24" s="19">
+        <v>0</v>
+      </c>
+      <c r="G24" s="19">
+        <v>250000</v>
+      </c>
+      <c r="H24" s="19">
+        <v>150000</v>
+      </c>
+      <c r="I24" s="19">
+        <v>0</v>
+      </c>
+      <c r="J24" s="19">
+        <v>300000</v>
+      </c>
+      <c r="K24" s="19">
+        <v>0</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="20">
+        <v>21</v>
+      </c>
+      <c r="D27" s="20">
+        <v>50</v>
+      </c>
+      <c r="E27" s="20">
+        <v>40</v>
+      </c>
+      <c r="F27" s="20">
+        <v>35</v>
+      </c>
+      <c r="G27" s="20">
+        <v>30</v>
+      </c>
+      <c r="H27" s="20">
+        <v>22</v>
+      </c>
+      <c r="I27" s="20">
+        <v>55</v>
+      </c>
+      <c r="J27" s="20">
+        <v>20</v>
+      </c>
+      <c r="K27" s="20">
+        <v>25</v>
+      </c>
+      <c r="L27" s="11"/>
+      <c r="M27" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="N27" s="3">
+        <f>SUMPRODUCT(C24:K24,C27:K27)</f>
+        <v>24000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="L30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="11">
+        <v>1</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11">
+        <v>1</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11">
+        <v>1</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31">
+        <f>SUMPRODUCT(C$24:K$24,C31:K31)</f>
+        <v>200000</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N31" s="11">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>180</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11">
+        <v>1</v>
+      </c>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11">
+        <v>1</v>
+      </c>
+      <c r="K32" s="11"/>
+      <c r="L32">
+        <f t="shared" ref="L32:L36" si="0">SUMPRODUCT(C$24:K$24,C32:K32)</f>
+        <v>550000</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N32" s="11">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11">
+        <v>1</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11">
+        <v>1</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>225000</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N33" s="11">
+        <v>225000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="11">
+        <v>1</v>
+      </c>
+      <c r="D34" s="11">
+        <v>1</v>
+      </c>
+      <c r="E34" s="11">
+        <v>1</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>275000</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="N34" s="11">
+        <v>275000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>184</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11">
+        <v>1</v>
+      </c>
+      <c r="G35" s="11">
+        <v>1</v>
+      </c>
+      <c r="H35" s="11">
+        <v>1</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>400000</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="N35" s="11">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>185</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11">
+        <v>1</v>
+      </c>
+      <c r="J36" s="11">
+        <v>1</v>
+      </c>
+      <c r="K36" s="11">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>300000</v>
+      </c>
+      <c r="M36" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="N36" s="11">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F6721C-D724-4FB3-BA26-AF745D479D1D}">
+  <dimension ref="A17:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="1">
+        <v>11.999999999999998</v>
+      </c>
+      <c r="D18" s="1">
+        <v>8.0000000000000018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="2">
+        <v>40</v>
+      </c>
+      <c r="D20" s="2">
+        <v>50</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="3">
+        <f>SUMPRODUCT(C18:D18,C20:D20)</f>
+        <v>880</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="11">
+        <f>SUMPRODUCT(C$18:D$18,C23:D23)</f>
+        <v>32</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" s="11">
+        <f>SUMPRODUCT(C$18:D$18,C24:D24)</f>
+        <v>48</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9827B3F-B8AB-4F9F-B69E-2140E77AD3B8}">
+  <dimension ref="A9:G19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="14">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="16">
+        <v>800</v>
+      </c>
+      <c r="D13" s="2">
+        <v>500</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="3">
+        <f>SUMPRODUCT(C10:D10,C13:D13)</f>
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="15">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <f>SUMPRODUCT(C$10:D$10,C16:D16)</f>
+        <v>80</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E19" si="0">SUMPRODUCT(C$10:D$10,C17:D17)</f>
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="15">
+        <v>-3</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>-150</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA431C68-A963-4032-A9E3-832D56096253}">
+  <dimension ref="A23:H33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="14">
+        <v>2.0000000000000027</v>
+      </c>
+      <c r="D24" s="14">
+        <v>8.9999999999999964</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="16">
+        <v>1200000</v>
+      </c>
+      <c r="D26" s="16">
+        <v>2000000</v>
+      </c>
+      <c r="E26" s="16">
+        <v>2600000</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26" s="17">
+        <f>SUMPRODUCT(C24:E24,C26:E26)</f>
+        <v>20399999.999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="15">
+        <v>4125000</v>
+      </c>
+      <c r="D30" s="15">
+        <v>8250000</v>
+      </c>
+      <c r="E30" s="15">
+        <v>12375000</v>
+      </c>
+      <c r="F30" s="15">
+        <f>SUMPRODUCT(C$24:E$24,C30:E30)</f>
+        <v>82499999.999999985</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="15">
+        <v>82500000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="15">
+        <v>30</v>
+      </c>
+      <c r="D31" s="15">
+        <v>15</v>
+      </c>
+      <c r="E31" s="15">
+        <v>45</v>
+      </c>
+      <c r="F31" s="15">
+        <f>SUMPRODUCT(C$24:E$24,C31:E31)</f>
+        <v>195.00000000000003</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="15">
+        <v>1</v>
+      </c>
+      <c r="D32" s="15">
+        <v>1</v>
+      </c>
+      <c r="E32" s="15">
+        <v>1</v>
+      </c>
+      <c r="F32" s="15">
+        <f>SUMPRODUCT(C24:E24,C32:E32)</f>
+        <v>11</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99904E52-0F97-453B-ACFC-A02604A71AB9}">
   <dimension ref="A3:P15"/>
   <sheetViews>
@@ -1817,7 +5189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA65B21-0A68-4A68-9A25-D1EA706A4FF7}">
   <dimension ref="L3:T37"/>
   <sheetViews>
@@ -2304,7 +5676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F0C024-D2F0-47AB-9D00-8587CB84FF8A}">
   <dimension ref="N3:V39"/>
   <sheetViews>
@@ -2811,4 +6183,505 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E64B88-1929-40D8-AF13-32396C61F2F0}">
+  <dimension ref="G17:M24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="17" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="1">
+        <v>10</v>
+      </c>
+      <c r="J18" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="2">
+        <v>300</v>
+      </c>
+      <c r="J20" s="2">
+        <v>400</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="M20" s="18">
+        <f>SUMPRODUCT(I18:J18,I20:J20)</f>
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="22" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>135</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <f>SUMPRODUCT(I$18:J$18,I23:J23)</f>
+        <v>80</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <f>SUMPRODUCT(I$18:J$18,I24:J24)</f>
+        <v>120</v>
+      </c>
+      <c r="L24" t="s">
+        <v>13</v>
+      </c>
+      <c r="M24">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3B02F0-729C-4C95-BE3C-36515FDB61E9}">
+  <dimension ref="M5:Y33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="Q5" t="s">
+        <v>198</v>
+      </c>
+      <c r="R5" t="s">
+        <v>199</v>
+      </c>
+      <c r="S5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="T6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="T7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>40</v>
+      </c>
+      <c r="R8">
+        <v>40</v>
+      </c>
+      <c r="S8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+    </row>
+    <row r="13" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="M13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="S13" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="T13" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="U13" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="M14" s="1"/>
+      <c r="N14" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="19">
+        <v>40</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>20</v>
+      </c>
+      <c r="R14" s="19">
+        <v>0</v>
+      </c>
+      <c r="S14" s="19">
+        <v>0</v>
+      </c>
+      <c r="T14" s="19">
+        <v>20</v>
+      </c>
+      <c r="U14" s="19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+    </row>
+    <row r="16" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+    </row>
+    <row r="17" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>195</v>
+      </c>
+      <c r="P17" s="20">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>6</v>
+      </c>
+      <c r="R17" s="20">
+        <v>4</v>
+      </c>
+      <c r="S17" s="20">
+        <v>6</v>
+      </c>
+      <c r="T17" s="20">
+        <v>5</v>
+      </c>
+      <c r="U17" s="20">
+        <v>2</v>
+      </c>
+      <c r="X17" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y17" s="22">
+        <f>SUMPRODUCT(P14:U14,P17:U17)</f>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="18" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+    </row>
+    <row r="19" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+    </row>
+    <row r="20" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="X20" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>196</v>
+      </c>
+      <c r="P21" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>1</v>
+      </c>
+      <c r="R21" s="11">
+        <v>1</v>
+      </c>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11">
+        <f>SUMPRODUCT(P$14:U$14,P21:U21)</f>
+        <v>60</v>
+      </c>
+      <c r="W21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="X21" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>197</v>
+      </c>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11">
+        <v>1</v>
+      </c>
+      <c r="T22" s="11">
+        <v>1</v>
+      </c>
+      <c r="U22" s="11">
+        <v>1</v>
+      </c>
+      <c r="V22" s="11">
+        <f t="shared" ref="V22:V25" si="0">SUMPRODUCT(P$14:U$14,P22:U22)</f>
+        <v>60</v>
+      </c>
+      <c r="W22" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="X22" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>201</v>
+      </c>
+      <c r="P23" s="11">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11">
+        <v>1</v>
+      </c>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="W23" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="X23" s="11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>202</v>
+      </c>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11">
+        <v>1</v>
+      </c>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11">
+        <v>1</v>
+      </c>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="W24" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="X24" s="11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>203</v>
+      </c>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11">
+        <v>1</v>
+      </c>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11">
+        <v>1</v>
+      </c>
+      <c r="V25" s="11">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="W25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="X25" s="11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+    </row>
+    <row r="27" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+    </row>
+    <row r="28" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+    </row>
+    <row r="29" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+    </row>
+    <row r="30" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+    </row>
+    <row r="31" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+    </row>
+    <row r="32" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+    </row>
+    <row r="33" spans="17:19" x14ac:dyDescent="0.25">
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>